<commit_message>
Cookie Checker Upload Compare and Send Email
</commit_message>
<xml_diff>
--- a/CookieChecker/Chrome-CookiesAccept.xlsx
+++ b/CookieChecker/Chrome-CookiesAccept.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10755" windowHeight="4935"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="48">
   <si>
     <t>Domain</t>
   </si>
@@ -833,7 +833,19 @@
         <v>26</v>
       </c>
       <c r="B18">
-        <v>0</v>
+        <v>4</v>
+      </c>
+      <c r="C18" t="s">
+        <v>6</v>
+      </c>
+      <c r="D18" t="s">
+        <v>9</v>
+      </c>
+      <c r="E18" t="s">
+        <v>3</v>
+      </c>
+      <c r="F18" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>